<commit_message>
added content on 28/12 sql
</commit_message>
<xml_diff>
--- a/DATASTAGE/invoice.xlsx
+++ b/DATASTAGE/invoice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MKM\SQL\For_SQL\DATASTAGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278D0B7D-12CF-4826-9448-084E918DF0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5828389-3344-4794-ADC6-77078244B629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0D413F8E-6908-4C43-B847-273E895E2450}"/>
   </bookViews>
@@ -19,16 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -238,7 +228,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,6 +248,13 @@
       <b/>
       <sz val="11"/>
       <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -307,20 +304,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -634,14 +635,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD0A17C-8140-4289-9A83-E59A2CA21B2B}">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="97" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -881,7 +882,7 @@
       <c r="J15" s="2">
         <v>5001</v>
       </c>
-      <c r="K15" s="5">
+      <c r="K15" s="2">
         <v>1</v>
       </c>
       <c r="L15" s="2">
@@ -928,7 +929,7 @@
       <c r="J16" s="2">
         <v>5001</v>
       </c>
-      <c r="K16" s="5">
+      <c r="K16" s="2">
         <v>2</v>
       </c>
       <c r="L16" s="2">
@@ -975,7 +976,7 @@
       <c r="J17" s="2">
         <v>5001</v>
       </c>
-      <c r="K17" s="5">
+      <c r="K17" s="2">
         <v>3</v>
       </c>
       <c r="L17" s="2">
@@ -1022,7 +1023,7 @@
       <c r="J18" s="2">
         <v>5002</v>
       </c>
-      <c r="K18" s="5">
+      <c r="K18" s="2">
         <v>1</v>
       </c>
       <c r="L18" s="2">
@@ -1069,7 +1070,7 @@
       <c r="J19" s="2">
         <v>5002</v>
       </c>
-      <c r="K19" s="5">
+      <c r="K19" s="2">
         <v>2</v>
       </c>
       <c r="L19" s="2">
@@ -1116,7 +1117,7 @@
       <c r="J20" s="2">
         <v>5003</v>
       </c>
-      <c r="K20" s="5">
+      <c r="K20" s="2">
         <v>1</v>
       </c>
       <c r="L20" s="2">
@@ -1149,7 +1150,7 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -1172,7 +1173,7 @@
       <c r="A26" s="2">
         <v>5001</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="2">
         <v>1</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -1187,7 +1188,7 @@
       <c r="H26" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="I26" s="7" t="s">
         <v>1</v>
       </c>
       <c r="J26" s="4" t="s">
@@ -1201,7 +1202,7 @@
       <c r="A27" s="2">
         <v>5001</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="2">
         <v>2</v>
       </c>
       <c r="C27" t="s">
@@ -1225,12 +1226,13 @@
       <c r="K27" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="M27" s="8"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>5001</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="2">
         <v>3</v>
       </c>
       <c r="C28" t="s">
@@ -1259,7 +1261,7 @@
       <c r="A29" s="2">
         <v>5002</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="2">
         <v>1</v>
       </c>
       <c r="C29" t="s">
@@ -1288,7 +1290,7 @@
       <c r="A30" s="2">
         <v>5002</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="2">
         <v>2</v>
       </c>
       <c r="C30" t="s">
@@ -1305,7 +1307,7 @@
       <c r="A31" s="2">
         <v>5003</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="2">
         <v>1</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -1337,10 +1339,10 @@
       </c>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E37" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G37" s="3" t="s">

</xml_diff>